<commit_message>
update fontawesome, affiliation and add orcid
</commit_message>
<xml_diff>
--- a/data/cv.xlsx
+++ b/data/cv.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="171">
   <si>
     <t>position</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>Head of the Biostatistic Team</t>
-  </si>
-  <si>
-    <t>[EGID - UMR 8199](http://www.good.cnrs.fr/?lang=en)</t>
   </si>
   <si>
     <t>Lille, France</t>
@@ -570,6 +567,27 @@
   </si>
   <si>
     <t>show</t>
+  </si>
+  <si>
+    <t>[EGID - UMR 1283](http://www.good.cnrs.fr/?lang=en)</t>
+  </si>
+  <si>
+    <t>Dec. 2019</t>
+  </si>
+  <si>
+    <t>Jan. 2020</t>
+  </si>
+  <si>
+    <t>Functional (Epi)genomics and Molecular  
+Physiology of Diabetes and Associated Diseases  
+EGID - UMR 1283  
+(European Genomics Institute for Diabetes)</t>
+  </si>
+  <si>
+    <t>orcid</t>
+  </si>
+  <si>
+    <t>0000-0002-3396-4549</t>
   </si>
 </sst>
 </file>
@@ -890,11 +908,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -903,12 +919,13 @@
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -925,39 +942,45 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G2" t="s">
         <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -981,84 +1004,84 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" t="s">
         <v>79</v>
-      </c>
-      <c r="E1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" t="s">
         <v>141</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>142</v>
       </c>
-      <c r="D2" t="s">
-        <v>143</v>
-      </c>
       <c r="E2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" t="s">
         <v>138</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>139</v>
       </c>
-      <c r="D3" t="s">
-        <v>140</v>
-      </c>
       <c r="E3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>136</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1083,27 +1106,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1111,7 +1134,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1122,13 +1145,13 @@
     </row>
     <row r="4" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1136,13 +1159,13 @@
     </row>
     <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1150,13 +1173,13 @@
     </row>
     <row r="6" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1181,130 +1204,130 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
         <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
         <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
         <v>30</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1327,79 +1350,79 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
         <v>35</v>
-      </c>
-      <c r="B1" t="s">
-        <v>36</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
         <v>37</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>38</v>
-      </c>
-      <c r="F1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
         <v>50</v>
       </c>
-      <c r="B2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>51</v>
-      </c>
-      <c r="E2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
         <v>45</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>46</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>47</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>48</v>
       </c>
-      <c r="E3" t="s">
-        <v>49</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
         <v>40</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>41</v>
       </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>42</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>43</v>
-      </c>
-      <c r="F4" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1409,10 +1432,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1436,93 +1459,93 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
         <v>37</v>
       </c>
-      <c r="E1" t="s">
-        <v>38</v>
-      </c>
       <c r="F1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
         <v>73</v>
       </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>74</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>75</v>
-      </c>
-      <c r="F2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
         <v>69</v>
       </c>
-      <c r="C3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>70</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>71</v>
-      </c>
-      <c r="F3" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
         <v>63</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>64</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>65</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>66</v>
-      </c>
-      <c r="F4" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>60</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>61</v>
-      </c>
-      <c r="F5" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1530,19 +1553,39 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
         <v>55</v>
       </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
+        <v>166</v>
+      </c>
+      <c r="F6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>167</v>
+      </c>
+      <c r="E7" t="s">
         <v>56</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F7" t="s">
         <v>57</v>
-      </c>
-      <c r="F6" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1570,10 +1613,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" t="s">
         <v>77</v>
-      </c>
-      <c r="B1" t="s">
-        <v>78</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1582,70 +1625,70 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" t="s">
         <v>79</v>
-      </c>
-      <c r="F1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
         <v>88</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E2" t="s">
-        <v>90</v>
-      </c>
       <c r="F2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
         <v>84</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>86</v>
       </c>
-      <c r="E3" t="s">
-        <v>87</v>
-      </c>
       <c r="F3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="s">
         <v>81</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>83</v>
-      </c>
       <c r="F4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1673,102 +1716,102 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
         <v>93</v>
       </c>
-      <c r="B1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>94</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>95</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>96</v>
-      </c>
-      <c r="F1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" t="s">
         <v>113</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>114</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
         <v>115</v>
-      </c>
-      <c r="D2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" t="s">
         <v>108</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>109</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>110</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
         <v>111</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s">
         <v>103</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>104</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>105</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
         <v>106</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" t="s">
         <v>98</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>99</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>100</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
         <v>101</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1794,7 +1837,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1803,33 +1846,33 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
         <v>79</v>
-      </c>
-      <c r="E1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" t="s">
         <v>118</v>
       </c>
-      <c r="C2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>119</v>
       </c>
-      <c r="E2" t="s">
-        <v>120</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1855,70 +1898,70 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" t="s">
         <v>79</v>
-      </c>
-      <c r="E1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>129</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>130</v>
-      </c>
       <c r="E2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" t="s">
         <v>126</v>
       </c>
-      <c r="D3" t="s">
-        <v>127</v>
-      </c>
       <c r="E3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" t="s">
         <v>122</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>123</v>
       </c>
-      <c r="D4" t="s">
-        <v>124</v>
-      </c>
       <c r="E4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix lab unit in short description
</commit_message>
<xml_diff>
--- a/data/cv.xlsx
+++ b/data/cv.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="1" r:id="rId1"/>
@@ -544,9 +544,6 @@
     <t>Data Analysis</t>
   </si>
   <si>
-    <t>I'm currently working for the *Institut Pasteur de Lille* at the *UMR 8199 - "Integrated Genomics and Metabolic Diseases Modelling"* as the *head of the biostatistic team*.</t>
-  </si>
-  <si>
     <t>I've been analysing omics (SNP, CpG, expression, metabolites, etc.) data within numerous projects related to metabolic diseases, such as Type 2 Diabetes.  
 These projects involve collaborations with national and international consortia like CKDgen, CHARGE, IMIDIA, DIRECT or more recently RHAPSODY.  
 My contribution covers Genome-Wide Association Studies (GWAS), differential methylation/expression analyses, metabolomics analyses, rare variants analyses (clustering approach), disease progression modelling, genetic epidemiology and meta-analyses.</t>
@@ -588,6 +585,9 @@
   </si>
   <si>
     <t>0000-0002-3396-4549</t>
+  </si>
+  <si>
+    <t>I'm currently working for the *Institut Pasteur de Lille* at the *UMR 1283 - "Functional (Epi)genomics and Molecular Physiology of Diabetes and Associated Diseases"* as the *head of the biostatistic team*.</t>
   </si>
 </sst>
 </file>
@@ -910,7 +910,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -942,7 +944,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -959,7 +961,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -971,7 +973,7 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -1093,8 +1095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,7 +1117,7 @@
         <v>155</v>
       </c>
       <c r="D1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1126,7 +1128,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1151,7 +1153,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1159,13 +1161,13 @@
     </row>
     <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1173,13 +1175,13 @@
     </row>
     <row r="6" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1562,7 +1564,7 @@
         <v>55</v>
       </c>
       <c r="E6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F6" t="s">
         <v>57</v>
@@ -1573,13 +1575,13 @@
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E7" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
add double number for institution and rename hex
</commit_message>
<xml_diff>
--- a/data/cv.xlsx
+++ b/data/cv.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="1" r:id="rId1"/>
@@ -561,9 +561,6 @@
     <t>show</t>
   </si>
   <si>
-    <t>[EGID - UMR 1283](http://www.good.cnrs.fr/?lang=en)</t>
-  </si>
-  <si>
     <t>Dec. 2019</t>
   </si>
   <si>
@@ -620,13 +617,16 @@
     <t xml:space="preserve">Mixed effects Score Test </t>
   </si>
   <si>
-    <t>I'm currently working for the *Institut Pasteur de Lille* at the *UMR 1283 - "Functional (Epi)genomics and Molecular Physiology of Diabetes and Related Diseases"* as the *head of the biostatistic team*.</t>
-  </si>
-  <si>
     <t>Functional (Epi)genomics and Molecular  
 Physiology of Diabetes and Related Diseases  
-EGID - UMR 1283  
+EGID - UMR 1283/8199  
 (European Genomics Institute for Diabetes)</t>
+  </si>
+  <si>
+    <t>I'm currently working for the *Institut Pasteur de Lille* at the *UMR 1283/8199 - "Functional (Epi)genomics and Molecular Physiology of Diabetes and Related Diseases"* as the *head of the biostatistic team*.</t>
+  </si>
+  <si>
+    <t>[EGID - UMR 1283/8199](http://www.good.cnrs.fr/?lang=en)</t>
   </si>
 </sst>
 </file>
@@ -949,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,7 +983,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -1000,7 +1000,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -1012,7 +1012,7 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -1135,7 +1135,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1443,7 +1443,7 @@
         <v>48</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1475,7 +1475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1571,7 +1571,7 @@
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>53</v>
@@ -1591,7 +1591,7 @@
     </row>
     <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>53</v>
@@ -1611,7 +1611,7 @@
     </row>
     <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>53</v>
@@ -1620,10 +1620,10 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F7" t="s">
         <v>56</v>
@@ -1631,16 +1631,16 @@
     </row>
     <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E8" t="s">
         <v>55</v>
@@ -1869,7 +1869,7 @@
         <v>99</v>
       </c>
       <c r="E5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F5" t="s">
         <v>100</v>
@@ -1877,13 +1877,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" t="s">
         <v>180</v>
       </c>
-      <c r="B6" t="s">
-        <v>181</v>
-      </c>
       <c r="C6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D6" t="s">
         <v>99</v>
@@ -1892,27 +1892,27 @@
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" t="s">
         <v>174</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>175</v>
-      </c>
-      <c r="C7" t="s">
-        <v>176</v>
       </c>
       <c r="D7" t="s">
         <v>99</v>
       </c>
       <c r="E7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add github link for clere
</commit_message>
<xml_diff>
--- a/data/cv.xlsx
+++ b/data/cv.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="183">
   <si>
     <t>position</t>
   </si>
@@ -378,9 +378,6 @@
   </si>
   <si>
     <t>Loïc Yengo, Julien Jacques, Christophe Biernacki and Mickaël Canouil</t>
-  </si>
-  <si>
-    <t>CRAN</t>
   </si>
   <si>
     <t>2014-02</t>
@@ -949,7 +946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -983,7 +980,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -1000,7 +997,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -1012,7 +1009,7 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -1048,7 +1045,7 @@
         <v>75</v>
       </c>
       <c r="B1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1062,67 +1059,67 @@
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" t="s">
         <v>139</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>140</v>
       </c>
-      <c r="D2" t="s">
-        <v>141</v>
-      </c>
       <c r="E2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" t="s">
         <v>136</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>137</v>
       </c>
-      <c r="D3" t="s">
-        <v>138</v>
-      </c>
       <c r="E3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1153,21 +1150,21 @@
         <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1175,7 +1172,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1186,13 +1183,13 @@
     </row>
     <row r="4" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1200,13 +1197,13 @@
     </row>
     <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1214,13 +1211,13 @@
     </row>
     <row r="6" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1443,7 +1440,7 @@
         <v>48</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1571,7 +1568,7 @@
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>53</v>
@@ -1591,7 +1588,7 @@
     </row>
     <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>53</v>
@@ -1611,7 +1608,7 @@
     </row>
     <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>53</v>
@@ -1620,10 +1617,10 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F7" t="s">
         <v>56</v>
@@ -1631,16 +1628,16 @@
     </row>
     <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E8" t="s">
         <v>55</v>
@@ -1709,7 +1706,7 @@
         <v>88</v>
       </c>
       <c r="F2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1729,7 +1726,7 @@
         <v>85</v>
       </c>
       <c r="F3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1740,7 +1737,7 @@
         <v>80</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -1749,7 +1746,7 @@
         <v>81</v>
       </c>
       <c r="F4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1761,8 +1758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1797,13 +1794,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" t="s">
         <v>111</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>112</v>
-      </c>
-      <c r="C2" t="s">
-        <v>113</v>
       </c>
       <c r="D2" t="s">
         <v>104</v>
@@ -1812,7 +1809,7 @@
         <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1826,13 +1823,13 @@
         <v>108</v>
       </c>
       <c r="D3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1869,7 +1866,7 @@
         <v>99</v>
       </c>
       <c r="E5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F5" t="s">
         <v>100</v>
@@ -1877,13 +1874,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B6" t="s">
         <v>179</v>
       </c>
-      <c r="B6" t="s">
-        <v>180</v>
-      </c>
       <c r="C6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D6" t="s">
         <v>99</v>
@@ -1892,27 +1889,27 @@
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B7" t="s">
         <v>173</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>174</v>
-      </c>
-      <c r="C7" t="s">
-        <v>175</v>
       </c>
       <c r="D7" t="s">
         <v>99</v>
       </c>
       <c r="E7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -1958,22 +1955,22 @@
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="C2" t="s">
         <v>84</v>
       </c>
       <c r="D2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" t="s">
         <v>117</v>
       </c>
-      <c r="E2" t="s">
-        <v>118</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2002,7 +1999,7 @@
         <v>75</v>
       </c>
       <c r="B1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2016,53 +2013,53 @@
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" t="s">
         <v>124</v>
       </c>
-      <c r="D3" t="s">
-        <v>125</v>
-      </c>
       <c r="E3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" t="s">
         <v>120</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>121</v>
       </c>
-      <c r="D4" t="s">
-        <v>122</v>
-      </c>
       <c r="E4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
title case; remove abstract field
</commit_message>
<xml_diff>
--- a/data/cv.xlsx
+++ b/data/cv.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="190">
   <si>
     <t>position</t>
   </si>
@@ -408,9 +408,6 @@
     <t>Project: *Detection of new genomic variants associated with fasting blood glucose and incidence of type 2 diabetes simultaneously*</t>
   </si>
   <si>
-    <t>Jointly Modelling SNPs with Survival &amp; Longitudinal Trait</t>
-  </si>
-  <si>
     <t>[A Statistical Seminar Applied on Type 2 Diabetes](https://www.med.lu.se/kalendarium/190121_canouil/)  
 (Host: Pr. Paul Franks)</t>
   </si>
@@ -434,9 +431,6 @@
     <t>Oct. 2018</t>
   </si>
   <si>
-    <t>Longitudinal Genetic Modelling: Revisiting Associations of SNPs Associated with Blood Fasting Glucose in Normoglycemic Individuals</t>
-  </si>
-  <si>
     <t>Statistical Methods for Post Genomic Data  
 (SMPGD)</t>
   </si>
@@ -639,6 +633,18 @@
   </si>
   <si>
     <t>briatte</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Contributor</t>
+  </si>
+  <si>
+    <t>Longitudinal Genetic Modelling: Revisiting Associations of SNPs Associated With Blood Fasting Glucose in Normoglycemic Individuals</t>
+  </si>
+  <si>
+    <t>Jointly Modelling SNPs With Survival &amp; Longitudinal Trait</t>
   </si>
 </sst>
 </file>
@@ -995,7 +1001,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -1012,7 +1018,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -1024,7 +1030,7 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -1045,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,7 +1066,7 @@
         <v>75</v>
       </c>
       <c r="B1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1074,67 +1080,67 @@
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" t="s">
         <v>138</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D2" t="s">
-        <v>140</v>
-      </c>
       <c r="E2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" t="s">
         <v>135</v>
       </c>
-      <c r="C3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D3" t="s">
-        <v>137</v>
-      </c>
       <c r="E3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1165,21 +1171,21 @@
         <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1187,7 +1193,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1198,13 +1204,13 @@
     </row>
     <row r="4" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1212,13 +1218,13 @@
     </row>
     <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1226,13 +1232,13 @@
     </row>
     <row r="6" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1455,7 +1461,7 @@
         <v>48</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1583,7 +1589,7 @@
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>53</v>
@@ -1603,7 +1609,7 @@
     </row>
     <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>53</v>
@@ -1623,7 +1629,7 @@
     </row>
     <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>53</v>
@@ -1632,10 +1638,10 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F7" t="s">
         <v>56</v>
@@ -1643,16 +1649,16 @@
     </row>
     <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E8" t="s">
         <v>55</v>
@@ -1721,7 +1727,7 @@
         <v>88</v>
       </c>
       <c r="F2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1741,7 +1747,7 @@
         <v>85</v>
       </c>
       <c r="F3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1752,7 +1758,7 @@
         <v>80</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -1761,7 +1767,7 @@
         <v>81</v>
       </c>
       <c r="F4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1771,10 +1777,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1782,12 +1788,13 @@
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="66.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>91</v>
       </c>
@@ -1798,16 +1805,19 @@
         <v>92</v>
       </c>
       <c r="D1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" t="s">
         <v>93</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>94</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>110</v>
       </c>
@@ -1818,16 +1828,19 @@
         <v>112</v>
       </c>
       <c r="D2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" t="s">
         <v>104</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>106</v>
       </c>
@@ -1838,16 +1851,19 @@
         <v>108</v>
       </c>
       <c r="D3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E3" t="s">
         <v>104</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -1858,16 +1874,19 @@
         <v>103</v>
       </c>
       <c r="D4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E4" t="s">
         <v>104</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>96</v>
       </c>
@@ -1878,73 +1897,85 @@
         <v>98</v>
       </c>
       <c r="D5" t="s">
+        <v>186</v>
+      </c>
+      <c r="E5" t="s">
         <v>99</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>169</v>
+      </c>
+      <c r="G5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C6" t="s">
+        <v>174</v>
+      </c>
+      <c r="D6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B7" t="s">
         <v>171</v>
       </c>
-      <c r="F5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>178</v>
-      </c>
-      <c r="B6" t="s">
-        <v>179</v>
-      </c>
-      <c r="C6" t="s">
-        <v>176</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D7" t="s">
+        <v>186</v>
+      </c>
+      <c r="E7" t="s">
         <v>99</v>
       </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>172</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="F7" t="s">
+        <v>169</v>
+      </c>
+      <c r="G7" t="s">
         <v>173</v>
       </c>
-      <c r="C7" t="s">
-        <v>174</v>
-      </c>
-      <c r="D7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" t="s">
-        <v>171</v>
-      </c>
-      <c r="F7" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D8" t="s">
+        <v>187</v>
+      </c>
+      <c r="E8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F8" t="s">
+        <v>185</v>
+      </c>
+      <c r="G8" t="s">
         <v>184</v>
-      </c>
-      <c r="B8" t="s">
-        <v>185</v>
-      </c>
-      <c r="C8" t="s">
-        <v>183</v>
-      </c>
-      <c r="D8" t="s">
-        <v>104</v>
-      </c>
-      <c r="E8" t="s">
-        <v>187</v>
-      </c>
-      <c r="F8" t="s">
-        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -2005,7 +2036,7 @@
         <v>117</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2018,7 +2049,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2034,7 +2065,7 @@
         <v>75</v>
       </c>
       <c r="B1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2048,53 +2079,53 @@
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>188</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>189</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" t="s">
         <v>123</v>
       </c>
-      <c r="D3" t="s">
-        <v>124</v>
-      </c>
       <c r="E3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" t="s">
         <v>119</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>120</v>
       </c>
-      <c r="D4" t="s">
-        <v>121</v>
-      </c>
       <c r="E4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor update for packages
</commit_message>
<xml_diff>
--- a/data/cv.xlsx
+++ b/data/cv.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="192">
   <si>
     <t>position</t>
   </si>
@@ -645,6 +645,12 @@
   </si>
   <si>
     <t>Jointly Modelling SNPs With Survival &amp; Longitudinal Trait</t>
+  </si>
+  <si>
+    <t>Author/Creator</t>
+  </si>
+  <si>
+    <t>Contributor/Creator</t>
   </si>
 </sst>
 </file>
@@ -1051,7 +1057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1779,7 +1785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1788,7 +1794,7 @@
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="66.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
@@ -1828,7 +1834,7 @@
         <v>112</v>
       </c>
       <c r="D2" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E2" t="s">
         <v>104</v>
@@ -1874,7 +1880,7 @@
         <v>103</v>
       </c>
       <c r="D4" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E4" t="s">
         <v>104</v>
@@ -1897,7 +1903,7 @@
         <v>98</v>
       </c>
       <c r="D5" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E5" t="s">
         <v>99</v>
@@ -1920,7 +1926,7 @@
         <v>174</v>
       </c>
       <c r="D6" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="E6" t="s">
         <v>99</v>
@@ -1943,7 +1949,7 @@
         <v>172</v>
       </c>
       <c r="D7" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E7" t="s">
         <v>99</v>

</xml_diff>

<commit_message>
change repo for rain
</commit_message>
<xml_diff>
--- a/data/cv.xlsx
+++ b/data/cv.xlsx
@@ -1786,7 +1786,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1955,7 +1955,7 @@
         <v>99</v>
       </c>
       <c r="F7" t="s">
-        <v>169</v>
+        <v>13</v>
       </c>
       <c r="G7" t="s">
         <v>173</v>

</xml_diff>

<commit_message>
minor text style changes
</commit_message>
<xml_diff>
--- a/data/cv.xlsx
+++ b/data/cv.xlsx
@@ -647,10 +647,10 @@
     <t>Jointly Modelling SNPs With Survival &amp; Longitudinal Trait</t>
   </si>
   <si>
-    <t>Author/Creator</t>
-  </si>
-  <si>
-    <t>Contributor/Creator</t>
+    <t>Author / Creator</t>
+  </si>
+  <si>
+    <t>Contributor / Creator</t>
   </si>
 </sst>
 </file>
@@ -1786,7 +1786,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add R packages (dmapaq, dgapaq, ggpacman)
</commit_message>
<xml_diff>
--- a/data/cv.xlsx
+++ b/data/cv.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11400" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="202">
   <si>
     <t>position</t>
   </si>
@@ -651,6 +651,36 @@
   </si>
   <si>
     <t>Contributor / Creator</t>
+  </si>
+  <si>
+    <t>ggpacman</t>
+  </si>
+  <si>
+    <t>A 'ggplot2' and 'gganimate' Version of Pac-Man</t>
+  </si>
+  <si>
+    <t>Mickaël Canouil</t>
+  </si>
+  <si>
+    <t>2020-05</t>
+  </si>
+  <si>
+    <t>2020-03</t>
+  </si>
+  <si>
+    <t>DNA Genotyping Arrays Processing And Quality-Control</t>
+  </si>
+  <si>
+    <t>dgapaq</t>
+  </si>
+  <si>
+    <t>dmapaq</t>
+  </si>
+  <si>
+    <t>DNA Methylation Arrays Processing And Quality-Control</t>
+  </si>
+  <si>
+    <t>Mickaël Canouil and Lijiao Ning</t>
   </si>
 </sst>
 </file>
@@ -1783,16 +1813,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="66.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
@@ -1984,8 +2014,78 @@
         <v>184</v>
       </c>
     </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B9" t="s">
+        <v>197</v>
+      </c>
+      <c r="C9" t="s">
+        <v>201</v>
+      </c>
+      <c r="D9" t="s">
+        <v>190</v>
+      </c>
+      <c r="E9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F9" t="s">
+        <v>169</v>
+      </c>
+      <c r="G9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>199</v>
+      </c>
+      <c r="B10" t="s">
+        <v>200</v>
+      </c>
+      <c r="C10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" t="s">
+        <v>190</v>
+      </c>
+      <c r="E10" t="s">
+        <v>99</v>
+      </c>
+      <c r="F10" t="s">
+        <v>169</v>
+      </c>
+      <c r="G10" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>192</v>
+      </c>
+      <c r="B11" t="s">
+        <v>193</v>
+      </c>
+      <c r="C11" t="s">
+        <v>194</v>
+      </c>
+      <c r="D11" t="s">
+        <v>190</v>
+      </c>
+      <c r="E11" t="s">
+        <v>104</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" t="s">
+        <v>195</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
reformat bib and fix typos
</commit_message>
<xml_diff>
--- a/data/cv.xlsx
+++ b/data/cv.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11400" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11400" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="204">
   <si>
     <t>position</t>
   </si>
@@ -63,9 +63,6 @@
     <t>twitter</t>
   </si>
   <si>
-    <t>Head of the Biostatistic Team</t>
-  </si>
-  <si>
     <t>Lille, France</t>
   </si>
   <si>
@@ -154,9 +151,6 @@
   </si>
   <si>
     <t>description</t>
-  </si>
-  <si>
-    <t>Doctor of Philosophy (Ph.D.) in BioStatistics</t>
   </si>
   <si>
     <t>University of Lille</t>
@@ -538,10 +532,6 @@
     <t>Team Management</t>
   </si>
   <si>
-    <t xml:space="preserve">I've been managing a team of three junior statisticians.  
-My role is to provide guidance regarding choices of statistical methodologies for analysing the data and code optimisation for implementing these methodologies in large scale omics data. </t>
-  </si>
-  <si>
     <t>Research</t>
   </si>
   <si>
@@ -573,12 +563,6 @@
   </si>
   <si>
     <t>Oct. 2017</t>
-  </si>
-  <si>
-    <t>Head of the Biostatistic Team (CNRS)</t>
-  </si>
-  <si>
-    <t>Head of the Biostatistic Team (Institut Pasteur de Lille)</t>
   </si>
   <si>
     <t>omicsr</t>
@@ -614,9 +598,6 @@
 (European Genomics Institute for Diabetes)</t>
   </si>
   <si>
-    <t>I'm currently working for the *Institut Pasteur de Lille* at the *UMR 1283/8199 - "Functional (Epi)genomics and Molecular Physiology of Diabetes and Related Diseases"* as the *head of the biostatistic team*.</t>
-  </si>
-  <si>
     <t>[EGID - UMR 1283/8199](http://www.good.cnrs.fr/?lang=en)</t>
   </si>
   <si>
@@ -681,6 +662,31 @@
   </si>
   <si>
     <t>Mickaël Canouil and Lijiao Ning</t>
+  </si>
+  <si>
+    <t>Head of the Biostatistics Team</t>
+  </si>
+  <si>
+    <t>I'm currently working for the *Institut Pasteur de Lille* at the *UMR 1283/8199 - "Functional (Epi)genomics and Molecular Physiology of Diabetes and Related Diseases"* as the *head of the biostatistics team*.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I've been managing a team of junior statisticians and interns . 
+My role is to provide guidance regarding choices of statistical methodologies for analysing the data and code optimisation for implementing these methodologies in large scale omics data. </t>
+  </si>
+  <si>
+    <t>rgroup</t>
+  </si>
+  <si>
+    <t>[R Lille - R User Group](https://rlille.github.io/)</t>
+  </si>
+  <si>
+    <t>Head of the Biostatistics Team (Institut Pasteur de Lille)</t>
+  </si>
+  <si>
+    <t>Head of the Biostatistics Team (CNRS)</t>
+  </si>
+  <si>
+    <t>Doctor of Philosophy (Ph.D.) in Biostatistics</t>
   </si>
 </sst>
 </file>
@@ -1001,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,7 +1026,7 @@
     <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1037,7 +1043,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -1048,34 +1054,40 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
-        <v>163</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
       <c r="I2" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -1099,84 +1111,84 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" t="s">
         <v>136</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D2" t="s">
-        <v>138</v>
-      </c>
       <c r="E2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" t="s">
         <v>133</v>
       </c>
-      <c r="C3" t="s">
-        <v>134</v>
-      </c>
-      <c r="D3" t="s">
-        <v>135</v>
-      </c>
       <c r="E3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
         <v>130</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
         <v>127</v>
       </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>129</v>
-      </c>
       <c r="E5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1189,7 +1201,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,27 +1213,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1229,7 +1241,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1240,13 +1252,13 @@
     </row>
     <row r="4" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1254,13 +1266,13 @@
     </row>
     <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>156</v>
+        <v>198</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1268,13 +1280,13 @@
     </row>
     <row r="6" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1299,130 +1311,130 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
         <v>29</v>
-      </c>
-      <c r="B13" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1434,8 +1446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1445,79 +1457,79 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
         <v>34</v>
-      </c>
-      <c r="B1" t="s">
-        <v>35</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>37</v>
-      </c>
-      <c r="F1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
         <v>49</v>
-      </c>
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
         <v>44</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>45</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>46</v>
       </c>
-      <c r="D3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" t="s">
-        <v>48</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>40</v>
       </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>41</v>
-      </c>
-      <c r="E4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1530,7 +1542,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1554,153 +1566,153 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
-        <v>37</v>
-      </c>
       <c r="F1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" t="s">
         <v>71</v>
       </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>72</v>
-      </c>
-      <c r="E2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="E3" t="s">
         <v>67</v>
       </c>
-      <c r="C3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>68</v>
-      </c>
-      <c r="E3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="s">
         <v>61</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>62</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>63</v>
-      </c>
-      <c r="E4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" t="s">
         <v>58</v>
-      </c>
-      <c r="E5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>202</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s">
         <v>54</v>
-      </c>
-      <c r="E6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>201</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>168</v>
+        <v>201</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1728,10 +1740,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1740,70 +1752,70 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" t="s">
         <v>86</v>
       </c>
-      <c r="B2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" t="s">
-        <v>88</v>
-      </c>
       <c r="F2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" t="s">
         <v>82</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" t="s">
-        <v>85</v>
-      </c>
       <c r="F3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
         <v>79</v>
       </c>
-      <c r="B4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>81</v>
-      </c>
       <c r="F4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1815,8 +1827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1832,255 +1844,255 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" t="s">
         <v>91</v>
       </c>
-      <c r="B1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>92</v>
       </c>
-      <c r="D1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>93</v>
-      </c>
-      <c r="F1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" t="s">
         <v>110</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>111</v>
-      </c>
-      <c r="C2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" t="s">
         <v>106</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
         <v>107</v>
-      </c>
-      <c r="C3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D3" t="s">
-        <v>186</v>
-      </c>
-      <c r="E3" t="s">
-        <v>104</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" t="s">
         <v>101</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
+        <v>184</v>
+      </c>
+      <c r="E4" t="s">
         <v>102</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
         <v>103</v>
-      </c>
-      <c r="D4" t="s">
-        <v>190</v>
-      </c>
-      <c r="E4" t="s">
-        <v>104</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" t="s">
         <v>96</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
+        <v>184</v>
+      </c>
+      <c r="E5" t="s">
         <v>97</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F5" t="s">
+        <v>164</v>
+      </c>
+      <c r="G5" t="s">
         <v>98</v>
-      </c>
-      <c r="D5" t="s">
-        <v>190</v>
-      </c>
-      <c r="E5" t="s">
-        <v>99</v>
-      </c>
-      <c r="F5" t="s">
-        <v>169</v>
-      </c>
-      <c r="G5" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B6" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C6" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D6" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B7" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C7" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D7" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="E7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B8" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D8" t="s">
         <v>181</v>
       </c>
-      <c r="D8" t="s">
-        <v>187</v>
-      </c>
       <c r="E8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F8" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="G8" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B9" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="C9" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="D9" t="s">
+        <v>184</v>
+      </c>
+      <c r="E9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" t="s">
+        <v>164</v>
+      </c>
+      <c r="G9" t="s">
         <v>190</v>
-      </c>
-      <c r="E9" t="s">
-        <v>99</v>
-      </c>
-      <c r="F9" t="s">
-        <v>169</v>
-      </c>
-      <c r="G9" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B10" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D10" t="s">
+        <v>184</v>
+      </c>
+      <c r="E10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" t="s">
+        <v>164</v>
+      </c>
+      <c r="G10" t="s">
         <v>190</v>
-      </c>
-      <c r="E10" t="s">
-        <v>99</v>
-      </c>
-      <c r="F10" t="s">
-        <v>169</v>
-      </c>
-      <c r="G10" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B11" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C11" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D11" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="E11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2107,7 +2119,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2116,33 +2128,33 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" t="s">
         <v>114</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" t="s">
         <v>115</v>
       </c>
-      <c r="C2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E2" t="s">
-        <v>117</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2168,70 +2180,70 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D3" t="s">
-        <v>123</v>
-      </c>
       <c r="E3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" t="s">
         <v>118</v>
       </c>
-      <c r="C4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D4" t="s">
-        <v>120</v>
-      </c>
       <c r="E4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update workshops and packages
</commit_message>
<xml_diff>
--- a/data/cv.xlsx
+++ b/data/cv.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11400" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7536" windowHeight="4392"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="skills" sheetId="2" r:id="rId3"/>
     <sheet name="education" sheetId="3" r:id="rId4"/>
     <sheet name="experience" sheetId="4" r:id="rId5"/>
-    <sheet name="teaching" sheetId="5" r:id="rId6"/>
+    <sheet name="workshop" sheetId="5" r:id="rId6"/>
     <sheet name="packages" sheetId="6" r:id="rId7"/>
     <sheet name="awards" sheetId="7" r:id="rId8"/>
     <sheet name="oral" sheetId="8" r:id="rId9"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="208">
   <si>
     <t>position</t>
   </si>
@@ -190,12 +190,6 @@
   </si>
   <si>
     <t>activities</t>
-  </si>
-  <si>
-    <t>Laboratory of Integrated Genomics  
-and Metabolic Diseases Modeling  
-EGID - UMR 8199  
-(European Genomics Institute for Diabetes)</t>
   </si>
   <si>
     <t>Jan. 2016</t>
@@ -283,41 +277,19 @@
     <t>Shiny: First Steps</t>
   </si>
   <si>
-    <t>One-day training (in French)</t>
-  </si>
-  <si>
     <t>Nov. 2019</t>
   </si>
   <si>
     <t>R and Databases</t>
   </si>
   <si>
-    <t>Two-days training (in French)</t>
-  </si>
-  <si>
     <t>Bordeaux, France</t>
   </si>
   <si>
     <t>May 2018</t>
   </si>
   <si>
-    <t>Julia for Intensive Scientific Computing</t>
-  </si>
-  <si>
     <t>Half-day workshop (in French)</t>
-  </si>
-  <si>
-    <t>Jul. 2015</t>
-  </si>
-  <si>
-    <t>"Unités Régionales de Formation  
-l'Information Scientifique et Technique"  
-(URFIST)</t>
-  </si>
-  <si>
-    <t>"Journées nationales du  
-DEVeloppement logiciel"  
-(JDEV)</t>
   </si>
   <si>
     <t>name</t>
@@ -480,38 +452,6 @@
 https://github.com/mcanouil/PRESENTATION/tree/master/SFD2015</t>
   </si>
   <si>
-    <t>https://github.com/mcanouil/PRESENTATION/tree/master/julia_tp</t>
-  </si>
-  <si>
-    <t>https://github.com/mcanouil/PRESENTATION/tree/5e439ff1db7f031c54f05d2cdcc6fbcfaeb21c32/rdatabase</t>
-  </si>
-  <si>
-    <t>https://github.com/mcanouil/rshiny/tree/edeca553c3c0905ae0d421cfa9099ad8435cc45e</t>
-  </si>
-  <si>
-    <t>https://github.com/mcanouil/PRESENTATION/tree/0b36aa0c679e07ffb448bb524ca06a20fd5779ae/joint_model</t>
-  </si>
-  <si>
-    <t>https://github.com/mcanouil/PRESENTATION/tree/dd43462ae2e8a21243296c175ddccc2c1887b3ad/joint_model</t>
-  </si>
-  <si>
-    <t>https://github.com/mcanouil/PRESENTATION/tree/master/SMPGD2016</t>
-  </si>
-  <si>
-    <t>https://github.com/mcanouil/PRESENTATION/tree/master/SFD2017</t>
-  </si>
-  <si>
-    <t>https://github.com/mcanouil/PRESENTATION/tree/master/IGES2016</t>
-  </si>
-  <si>
-    <t>https://github.com/mcanouil/PRESENTATION/tree/master/IGES2015</t>
-  </si>
-  <si>
-    <t>"Réseau Interdisciplinaire  
-autour de la Statistique" 
-(RIS)</t>
-  </si>
-  <si>
     <t>Curriculum Vitæ</t>
   </si>
   <si>
@@ -592,101 +532,167 @@
     <t xml:space="preserve">Mixed effects Score Test </t>
   </si>
   <si>
+    <t>François Briatte, Michał Bojanowski, Mickaël Canouil, Zachary Charlop-Powers, Jacob C. Fisher, Kipp Johnson and Tyler Rinker</t>
+  </si>
+  <si>
+    <t>ggnetwork</t>
+  </si>
+  <si>
+    <t>Geometries to Plot Networks with 'ggplot2'</t>
+  </si>
+  <si>
+    <t>2020-02</t>
+  </si>
+  <si>
+    <t>briatte</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Contributor</t>
+  </si>
+  <si>
+    <t>Longitudinal Genetic Modelling: Revisiting Associations of SNPs Associated With Blood Fasting Glucose in Normoglycemic Individuals</t>
+  </si>
+  <si>
+    <t>Jointly Modelling SNPs With Survival &amp; Longitudinal Trait</t>
+  </si>
+  <si>
+    <t>Author / Creator</t>
+  </si>
+  <si>
+    <t>Contributor / Creator</t>
+  </si>
+  <si>
+    <t>ggpacman</t>
+  </si>
+  <si>
+    <t>A 'ggplot2' and 'gganimate' Version of Pac-Man</t>
+  </si>
+  <si>
+    <t>Mickaël Canouil</t>
+  </si>
+  <si>
+    <t>2020-05</t>
+  </si>
+  <si>
+    <t>2020-03</t>
+  </si>
+  <si>
+    <t>DNA Genotyping Arrays Processing And Quality-Control</t>
+  </si>
+  <si>
+    <t>dgapaq</t>
+  </si>
+  <si>
+    <t>dmapaq</t>
+  </si>
+  <si>
+    <t>DNA Methylation Arrays Processing And Quality-Control</t>
+  </si>
+  <si>
+    <t>Mickaël Canouil and Lijiao Ning</t>
+  </si>
+  <si>
+    <t>Head of the Biostatistics Team</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I've been managing a team of junior statisticians and interns . 
+My role is to provide guidance regarding choices of statistical methodologies for analysing the data and code optimisation for implementing these methodologies in large scale omics data. </t>
+  </si>
+  <si>
+    <t>rgroup</t>
+  </si>
+  <si>
+    <t>[R Lille - R User Group](https://rlille.github.io/)</t>
+  </si>
+  <si>
+    <t>Head of the Biostatistics Team (Institut Pasteur de Lille)</t>
+  </si>
+  <si>
+    <t>Head of the Biostatistics Team (CNRS)</t>
+  </si>
+  <si>
+    <t>Doctor of Philosophy (Ph.D.) in Biostatistics</t>
+  </si>
+  <si>
+    <t>I'm currently working for the *Institut Pasteur de Lille* at the *INSERM U1283 / CNRS UMR 8199 - "Functional (Epi)genomics and Molecular Physiology of Diabetes and Related Diseases"* as the *head of the biostatistics team*.</t>
+  </si>
+  <si>
+    <t>Laboratory of Integrated Genomics  
+and Metabolic Diseases Modeling  
+CNRS UMR 8199 - EGID  
+(European Genomics Institute for Diabetes)</t>
+  </si>
+  <si>
     <t>Functional (Epi)genomics and Molecular  
 Physiology of Diabetes and Related Diseases  
-EGID - UMR 1283/8199  
+INSERM U1283 / CNRS UMR 8199 - EGID  
 (European Genomics Institute for Diabetes)</t>
   </si>
   <si>
-    <t>[EGID - UMR 1283/8199](http://www.good.cnrs.fr/?lang=en)</t>
-  </si>
-  <si>
-    <t>François Briatte, Michał Bojanowski, Mickaël Canouil, Zachary Charlop-Powers, Jacob C. Fisher, Kipp Johnson and Tyler Rinker</t>
-  </si>
-  <si>
-    <t>ggnetwork</t>
-  </si>
-  <si>
-    <t>Geometries to Plot Networks with 'ggplot2'</t>
-  </si>
-  <si>
-    <t>2020-02</t>
-  </si>
-  <si>
-    <t>briatte</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
-    <t>Contributor</t>
-  </si>
-  <si>
-    <t>Longitudinal Genetic Modelling: Revisiting Associations of SNPs Associated With Blood Fasting Glucose in Normoglycemic Individuals</t>
-  </si>
-  <si>
-    <t>Jointly Modelling SNPs With Survival &amp; Longitudinal Trait</t>
-  </si>
-  <si>
-    <t>Author / Creator</t>
-  </si>
-  <si>
-    <t>Contributor / Creator</t>
-  </si>
-  <si>
-    <t>ggpacman</t>
-  </si>
-  <si>
-    <t>A 'ggplot2' and 'gganimate' Version of Pac-Man</t>
-  </si>
-  <si>
-    <t>Mickaël Canouil</t>
-  </si>
-  <si>
-    <t>2020-05</t>
-  </si>
-  <si>
-    <t>2020-03</t>
-  </si>
-  <si>
-    <t>DNA Genotyping Arrays Processing And Quality-Control</t>
-  </si>
-  <si>
-    <t>dgapaq</t>
-  </si>
-  <si>
-    <t>dmapaq</t>
-  </si>
-  <si>
-    <t>DNA Methylation Arrays Processing And Quality-Control</t>
-  </si>
-  <si>
-    <t>Mickaël Canouil and Lijiao Ning</t>
-  </si>
-  <si>
-    <t>Head of the Biostatistics Team</t>
-  </si>
-  <si>
-    <t>I'm currently working for the *Institut Pasteur de Lille* at the *UMR 1283/8199 - "Functional (Epi)genomics and Molecular Physiology of Diabetes and Related Diseases"* as the *head of the biostatistics team*.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I've been managing a team of junior statisticians and interns . 
-My role is to provide guidance regarding choices of statistical methodologies for analysing the data and code optimisation for implementing these methodologies in large scale omics data. </t>
-  </si>
-  <si>
-    <t>rgroup</t>
-  </si>
-  <si>
-    <t>[R Lille - R User Group](https://rlille.github.io/)</t>
-  </si>
-  <si>
-    <t>Head of the Biostatistics Team (Institut Pasteur de Lille)</t>
-  </si>
-  <si>
-    <t>Head of the Biostatistics Team (CNRS)</t>
-  </si>
-  <si>
-    <t>Doctor of Philosophy (Ph.D.) in Biostatistics</t>
+    <t>R Advanced</t>
+  </si>
+  <si>
+    <t>Nov. 2020</t>
+  </si>
+  <si>
+    <t>ggplot2</t>
+  </si>
+  <si>
+    <t>Oct. 2020</t>
+  </si>
+  <si>
+    <t>https://github.com/mcanouil/rdatabase/</t>
+  </si>
+  <si>
+    <t>https://github.com/mcanouil/radvanced/</t>
+  </si>
+  <si>
+    <t>https://github.com/mcanouil/rshiny/</t>
+  </si>
+  <si>
+    <t>https://github.com/mcanouil/mctrainings/</t>
+  </si>
+  <si>
+    <t>https://github.com/mcanouil/rstartup/</t>
+  </si>
+  <si>
+    <t>One-day workshop (in French)</t>
+  </si>
+  <si>
+    <t>Two-days workshop (in French)</t>
+  </si>
+  <si>
+    <t>R Statup</t>
+  </si>
+  <si>
+    <t>insane</t>
+  </si>
+  <si>
+    <t>Feb. 2020</t>
+  </si>
+  <si>
+    <t>https://github.com/mcanouil/rpackages/</t>
+  </si>
+  <si>
+    <t>R Packages</t>
+  </si>
+  <si>
+    <t>Thirty minutes introduction (in French)</t>
+  </si>
+  <si>
+    <t>An Interactive Web Application for Quality Control and Analysis of Insulin Secretion from Pancreatic Beta Cells</t>
+  </si>
+  <si>
+    <t>2020-11</t>
+  </si>
+  <si>
+    <t>Thirty minutes overview (in English</t>
+  </si>
+  <si>
+    <t>[INSERM 1283 / CNRS 8199](http://www.good.cnrs.fr/?lang=en)</t>
   </si>
 </sst>
 </file>
@@ -1009,24 +1015,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1043,7 +1049,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -1055,15 +1061,15 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>207</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -1075,7 +1081,7 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -1087,7 +1093,7 @@
         <v>11</v>
       </c>
       <c r="J2" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -1100,95 +1106,86 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" t="s">
         <v>75</v>
       </c>
-      <c r="E1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C2" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C3" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>127</v>
-      </c>
-      <c r="E5" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1201,47 +1198,47 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="67.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="67.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
         <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="D1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1250,43 +1247,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1303,13 +1300,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1317,7 +1314,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1325,7 +1322,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1333,7 +1330,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1341,7 +1338,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1349,7 +1346,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1357,7 +1354,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1365,7 +1362,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1373,7 +1370,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1381,7 +1378,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1389,7 +1386,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1397,7 +1394,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1405,7 +1402,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1413,7 +1410,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1421,7 +1418,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1429,7 +1426,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1446,16 +1443,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="142.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="142.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1475,7 +1472,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1492,7 +1489,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1509,12 +1506,12 @@
         <v>46</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
@@ -1542,20 +1539,20 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="50" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="117.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="117.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1575,144 +1572,144 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
       </c>
       <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
         <v>70</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>71</v>
       </c>
-      <c r="F2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="C3" t="s">
         <v>44</v>
       </c>
       <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
         <v>66</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>67</v>
       </c>
-      <c r="F3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
         <v>59</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>60</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>61</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>62</v>
       </c>
-      <c r="F4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>51</v>
+        <v>185</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" t="s">
         <v>56</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>57</v>
       </c>
-      <c r="F5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>51</v>
+        <v>185</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E6" t="s">
         <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>51</v>
+        <v>185</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="E7" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="F7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" t="s">
         <v>53</v>
-      </c>
-      <c r="F8" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1722,100 +1719,138 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="131" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="131" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" t="s">
         <v>73</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>74</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
       </c>
       <c r="E1" t="s">
         <v>75</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>80</v>
-      </c>
       <c r="B3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>200</v>
+      </c>
+      <c r="E4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" t="s">
-        <v>140</v>
+      <c r="D6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>188</v>
+      </c>
+      <c r="E7" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -1825,274 +1860,297 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" t="s">
         <v>73</v>
       </c>
-      <c r="C1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D1" t="s">
-        <v>74</v>
-      </c>
       <c r="E1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D2" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="E2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D3" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="E3" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D4" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="E4" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D5" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="E5" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F5" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="G5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="B6" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="C6" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="D6" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="E6" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D7" t="s">
         <v>165</v>
       </c>
-      <c r="B7" t="s">
-        <v>166</v>
-      </c>
-      <c r="C7" t="s">
-        <v>167</v>
-      </c>
-      <c r="D7" t="s">
-        <v>184</v>
-      </c>
       <c r="E7" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F7" t="s">
         <v>12</v>
       </c>
       <c r="G7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" t="s">
+        <v>162</v>
+      </c>
+      <c r="E8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" t="s">
+        <v>160</v>
+      </c>
+      <c r="G8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C9" t="s">
+        <v>176</v>
+      </c>
+      <c r="D9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" t="s">
+        <v>147</v>
+      </c>
+      <c r="G9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B10" t="s">
+        <v>175</v>
+      </c>
+      <c r="C10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" t="s">
+        <v>165</v>
+      </c>
+      <c r="E10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" t="s">
+        <v>147</v>
+      </c>
+      <c r="G10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>167</v>
+      </c>
+      <c r="B11" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>176</v>
-      </c>
-      <c r="B8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C8" t="s">
-        <v>175</v>
-      </c>
-      <c r="D8" t="s">
-        <v>181</v>
-      </c>
-      <c r="E8" t="s">
-        <v>102</v>
-      </c>
-      <c r="F8" t="s">
-        <v>179</v>
-      </c>
-      <c r="G8" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>192</v>
-      </c>
-      <c r="B9" t="s">
-        <v>191</v>
-      </c>
-      <c r="C9" t="s">
-        <v>195</v>
-      </c>
-      <c r="D9" t="s">
-        <v>184</v>
-      </c>
-      <c r="E9" t="s">
-        <v>97</v>
-      </c>
-      <c r="F9" t="s">
-        <v>164</v>
-      </c>
-      <c r="G9" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>193</v>
-      </c>
-      <c r="B10" t="s">
-        <v>194</v>
-      </c>
-      <c r="C10" t="s">
-        <v>96</v>
-      </c>
-      <c r="D10" t="s">
-        <v>184</v>
-      </c>
-      <c r="E10" t="s">
-        <v>97</v>
-      </c>
-      <c r="F10" t="s">
-        <v>164</v>
-      </c>
-      <c r="G10" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>186</v>
-      </c>
-      <c r="B11" t="s">
-        <v>187</v>
-      </c>
       <c r="C11" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="D11" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="E11" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="F11" t="s">
         <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>189</v>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>199</v>
+      </c>
+      <c r="B12" t="s">
+        <v>204</v>
+      </c>
+      <c r="C12" t="s">
+        <v>169</v>
+      </c>
+      <c r="D12" t="s">
+        <v>165</v>
+      </c>
+      <c r="E12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -2109,17 +2167,17 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="99.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="99.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2128,33 +2186,33 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E1" t="s">
         <v>37</v>
       </c>
       <c r="F1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2167,83 +2225,74 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" customWidth="1"/>
-    <col min="2" max="2" width="60.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.88671875" customWidth="1"/>
+    <col min="2" max="2" width="60.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" t="s">
         <v>75</v>
       </c>
-      <c r="E1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C4" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E4" t="s">
-        <v>141</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>